<commit_message>
feat: add full BE (FastAPI) + FE (Streamlit) pipeline, TTL/cleanup, health-check, merge/zip
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -7,52 +7,31 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Mẫu số" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="39">
-  <si>
-    <t>Mẫu số</t>
-  </si>
-  <si>
-    <t>KH hóa đơn</t>
-  </si>
-  <si>
-    <t>Số hóa đơn</t>
-  </si>
-  <si>
-    <t>ngày hóa đơn</t>
-  </si>
-  <si>
-    <t>ST người bán</t>
-  </si>
-  <si>
-    <t>tên người bán</t>
-  </si>
-  <si>
-    <t>C người bán</t>
-  </si>
-  <si>
-    <t>Mã hàng</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+  <si>
+    <t>Cờ (Tchat)</t>
   </si>
   <si>
     <t>Tên hàng</t>
   </si>
   <si>
-    <t>Đơn vị tính</t>
-  </si>
-  <si>
-    <t>Số lượng</t>
+    <t>ĐVT</t>
+  </si>
+  <si>
+    <t>SL</t>
   </si>
   <si>
     <t>Đơn giá</t>
   </si>
   <si>
-    <t>Tiền hàng</t>
+    <t>Thành tiền</t>
   </si>
   <si>
     <t>Thuế suất</t>
@@ -64,73 +43,31 @@
     <t>Cộng tiền</t>
   </si>
   <si>
+    <t>Đơn vị tiền</t>
+  </si>
+  <si>
+    <t>Tỷ giá</t>
+  </si>
+  <si>
     <t>Ghi chú</t>
   </si>
   <si>
-    <t>Đơn vị tiền</t>
-  </si>
-  <si>
-    <t>Tỷ giá</t>
-  </si>
-  <si>
-    <t>Cờ (Tchat)</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>C25TLT</t>
-  </si>
-  <si>
-    <t>00003000</t>
-  </si>
-  <si>
-    <t>2025-10-29</t>
-  </si>
-  <si>
-    <t>0312637362</t>
-  </si>
-  <si>
-    <t>CÔNG TY TNHH XUẤT NHẬP KHẨU THƯƠNG MẠI LINH THÀNH</t>
-  </si>
-  <si>
-    <t>21/21 Lê Duy Nhuận, Phường Bảy Hiền, Thành phố Hồ Chí Minh, Việt Nam</t>
-  </si>
-  <si>
-    <t>VBCN</t>
-  </si>
-  <si>
-    <t>KOY_28985/20</t>
-  </si>
-  <si>
-    <t>NTN_30207JR</t>
-  </si>
-  <si>
-    <t>KOY_5210-2RS</t>
+    <t>Nguồn (file)</t>
+  </si>
+  <si>
+    <t>4</t>
   </si>
   <si>
     <t>Vòng bi công nghiệp mới 100%</t>
   </si>
   <si>
-    <t>KOYO 28985/20</t>
-  </si>
-  <si>
-    <t>NTN 30207</t>
-  </si>
-  <si>
-    <t>KOYO 52102RS</t>
-  </si>
-  <si>
-    <t>Cái</t>
+    <t>VND</t>
   </si>
   <si>
     <t>Hoá đơn mới</t>
   </si>
   <si>
-    <t>VND</t>
-  </si>
-  <si>
-    <t>4</t>
+    <t>input.xml</t>
   </si>
 </sst>
 </file>
@@ -488,13 +425,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T5"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -534,268 +471,43 @@
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="B2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0.08</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="M2" t="s">
         <v>17</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20">
-      <c r="A2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I2" t="s">
-        <v>31</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>36</v>
-      </c>
-      <c r="R2" t="s">
-        <v>37</v>
-      </c>
-      <c r="S2">
-        <v>1</v>
-      </c>
-      <c r="T2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I3" t="s">
-        <v>32</v>
-      </c>
-      <c r="J3" t="s">
-        <v>35</v>
-      </c>
-      <c r="K3">
-        <v>6</v>
-      </c>
-      <c r="L3">
-        <v>277777.78</v>
-      </c>
-      <c r="M3">
-        <v>1666667</v>
-      </c>
-      <c r="N3">
-        <v>0.08</v>
-      </c>
-      <c r="O3">
-        <v>133333</v>
-      </c>
-      <c r="P3">
-        <v>1800000</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>36</v>
-      </c>
-      <c r="R3" t="s">
-        <v>37</v>
-      </c>
-      <c r="S3">
-        <v>1</v>
-      </c>
-      <c r="T3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" t="s">
-        <v>29</v>
-      </c>
-      <c r="I4" t="s">
-        <v>33</v>
-      </c>
-      <c r="J4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K4">
-        <v>10</v>
-      </c>
-      <c r="L4">
-        <v>106481.48</v>
-      </c>
-      <c r="M4">
-        <v>1064815</v>
-      </c>
-      <c r="N4">
-        <v>0.08</v>
-      </c>
-      <c r="O4">
-        <v>85185</v>
-      </c>
-      <c r="P4">
-        <v>1150000</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>36</v>
-      </c>
-      <c r="R4" t="s">
-        <v>37</v>
-      </c>
-      <c r="S4">
-        <v>1</v>
-      </c>
-      <c r="T4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" t="s">
-        <v>34</v>
-      </c>
-      <c r="J5" t="s">
-        <v>35</v>
-      </c>
-      <c r="K5">
-        <v>3</v>
-      </c>
-      <c r="L5">
-        <v>611111.11</v>
-      </c>
-      <c r="M5">
-        <v>1833333</v>
-      </c>
-      <c r="N5">
-        <v>0.08</v>
-      </c>
-      <c r="O5">
-        <v>146667</v>
-      </c>
-      <c r="P5">
-        <v>1980000</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>36</v>
-      </c>
-      <c r="R5" t="s">
-        <v>37</v>
-      </c>
-      <c r="S5">
-        <v>1</v>
-      </c>
-      <c r="T5" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>